<commit_message>
Solving uploading issues with the server (OneDrive).
</commit_message>
<xml_diff>
--- a/Datos/data_implementation.xlsx
+++ b/Datos/data_implementation.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://psmhs.sharepoint.com/sites/Computer-Assisted-Reading-Interventions/Shared Documents/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{0F924EF0-CB86-2A48-A807-4FA2CDBF7861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D4B0A45A-4B0F-2342-836A-061C25843B24}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{0F924EF0-CB86-2A48-A807-4FA2CDBF7861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{92887311-0006-914B-8B75-2BA7B8A32746}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="_56F9DC9755BA473782653E2940F9" sheetId="2" state="veryHidden" r:id="rId1"/>
-    <sheet name="Form1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="_56F9DC9755BA473782653E2940F9" sheetId="2" state="veryHidden" r:id="rId2"/>
+    <sheet name="Form1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_56F9DC9755BA473782653E2940F9FormId">"wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu"</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="261">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -51,12 +52,24 @@
     <t>Callaghan et al</t>
   </si>
   <si>
+    <t>Phonological skills</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
     <t>Individual</t>
   </si>
   <si>
+    <t>Lexia Reading Core 5 (Lexia)</t>
+  </si>
+  <si>
+    <t>Phonological Assessment Battery Second Edition (PhAB-2)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Cazzell et al</t>
   </si>
   <si>
@@ -66,12 +79,27 @@
     <t>3</t>
   </si>
   <si>
+    <t xml:space="preserve">No reportaron estadísticas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both participants did rapidly acquire words after the intervention was applied. Nevertheless, the authors mention that the increases in word-reading performance may have been caused by testing effects. </t>
+  </si>
+  <si>
     <t>Chai</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
+    <t>Touch Sound</t>
+  </si>
+  <si>
+    <t>All children in the current study not only improved performance on their own target phonemes but also learned a portion of other children’s target phonemes through observation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No se presentaron estadísticas descriptivas ni inferenciales. </t>
+  </si>
+  <si>
     <t>Comaskey et al</t>
   </si>
   <si>
@@ -81,36 +109,117 @@
     <t>4</t>
   </si>
   <si>
+    <t>A Balanced Reading Approach for Canadians Designed to Achieve Best Results for All (ABRACADABRA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peabody Picture Vocabulary Test (PPVT), Letter-sound knowledge, Wide Range Achievement Test Word Recognition Subtest, Segmenting and Blending, Common units tasks, Nonsense word recognition, Unique word recognition. </t>
+  </si>
+  <si>
+    <t>ANCOVA</t>
+  </si>
+  <si>
     <t>Moser et al</t>
   </si>
   <si>
+    <t>8 great word patters</t>
+  </si>
+  <si>
+    <t>Rate (wpm) and accuracy of results</t>
+  </si>
+  <si>
+    <t>Analysis of Covariance (ANCOVA) was only used for comprehension, vocabulary; only descriptive statistics were provided for other variables</t>
+  </si>
+  <si>
+    <t>Comprehension almost reached statistical significance (0.13), Vocabulary almost reached statistical significance (0.07). 
+There are some problems with the presentation of results. It seems that the DRA2 was analyzed in 2 ways (it is unclear) because the authors reference the same skills but provide different "results" and interpretations and they don't describe the instrument in detail.
+Most instruments were not described in detail so it is hard to determine improvements.
+All differences were very modest.</t>
+  </si>
+  <si>
     <t>Pindiprolu et al</t>
   </si>
   <si>
+    <t>Funnix and Headsprout</t>
+  </si>
+  <si>
+    <t>Dynamic Indicators of Basic Early Literacy Skills (DIBELS)</t>
+  </si>
+  <si>
+    <t>Adjusted means</t>
+  </si>
+  <si>
     <t>Potocki et al</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
+    <t>Chassymo, Locotex</t>
+  </si>
+  <si>
+    <t>Timé3, Alouette, Semantic similarity judgment task, name for measuring reading comprehension was not provided</t>
+  </si>
+  <si>
+    <t>specific p-values were only provided for nonsignificant statistical results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The authors were interested in comparing the effects of two interventions focused on different skills and some of the results were of the interaction. The results for the pretest-posttest alone were not always provided. </t>
+  </si>
+  <si>
     <t>27</t>
   </si>
   <si>
+    <t>GraphoGame</t>
+  </si>
+  <si>
+    <t>Not specified (instruments seemed to have been designed by the researchers)</t>
+  </si>
+  <si>
     <t>Saine et al</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
+    <t>Lukilasse Graded Fluency Test</t>
+  </si>
+  <si>
+    <t>Groups were balanced on pretest-reading skills</t>
+  </si>
+  <si>
+    <t>min, max</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
     <t>Schmitt et al</t>
   </si>
   <si>
     <t>Not reported</t>
   </si>
   <si>
+    <t>Phonological Awareness Literacy Screening PreK assessment, Get Ready to Read!-Revised, researcher-developed measures</t>
+  </si>
+  <si>
+    <t>All the parent's variables were integrated into a composite score. Specific p-values were reported for nonsignificant results</t>
+  </si>
+  <si>
     <t>45</t>
   </si>
   <si>
+    <t>ceiling effects</t>
+  </si>
+  <si>
+    <t>The covariate was inferred based on the description; these seem to be very rigorous but I can't be sure because I don't know them enough</t>
+  </si>
+  <si>
+    <t>The authors provided CI for effect size and these were very wide, which was acknowledged by the authors</t>
+  </si>
+  <si>
+    <t>Very nice study but complicated because of very specialized statistical analysis</t>
+  </si>
+  <si>
     <t>Ecalle et al</t>
   </si>
   <si>
@@ -120,21 +229,66 @@
     <t>Wood et al</t>
   </si>
   <si>
+    <t>Dynamic Indicators of Basic Early Literacy Skills</t>
+  </si>
+  <si>
+    <t>This was a SSD</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
+    <t>Word reading aloud task</t>
+  </si>
+  <si>
     <t>Kyle et al</t>
   </si>
   <si>
+    <t>Only the intervention groups were balanced (not the control group)</t>
+  </si>
+  <si>
+    <t>The presentation of p-values was inconsistent. Only the p-values approaching significance level were presented.</t>
+  </si>
+  <si>
+    <t>All p-values were very close to reaching statistical significance (e.g., p-value = .06), but due to how effectiveness was defined, the results were considered nonsignificant and the intervention not effective</t>
+  </si>
+  <si>
     <t>Fan et al</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
+    <t>PhonoBlocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Six rule-based lessons </t>
+  </si>
+  <si>
+    <t>t-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descriptive data was presented in narrative (only the mean of raw scores). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data was presented in narrative (didn't use tables). </t>
+  </si>
+  <si>
     <t>Kleinsz et al</t>
   </si>
   <si>
+    <t>Grapho-syllabic training, Comprehension training (CoT).</t>
+  </si>
+  <si>
+    <t>Wilcoxon signed-rank test</t>
+  </si>
+  <si>
+    <t>Wilcoxon analyses were conducted because of sample size</t>
+  </si>
+  <si>
+    <t>Many statistical analyses were conducted</t>
+  </si>
+  <si>
     <t>Gustafson et al</t>
   </si>
   <si>
@@ -144,6 +298,24 @@
     <t>60</t>
   </si>
   <si>
+    <t xml:space="preserve">Oxford Reading Tree (ORT) for Clicker </t>
+  </si>
+  <si>
+    <t>Lexical decision task (LDT), Single word oral reading task (SWORT), and Phonological Awareness Test (PAT).</t>
+  </si>
+  <si>
+    <t>trainertext</t>
+  </si>
+  <si>
+    <t>Working Memory Test Battery for Children</t>
+  </si>
+  <si>
+    <t>TOWRE, Phonological Assessment Battery, PhAB, BAS II Spelling Scale</t>
+  </si>
+  <si>
+    <t>general ability (IQ)</t>
+  </si>
+  <si>
     <t>2 - 3</t>
   </si>
   <si>
@@ -153,12 +325,54 @@
     <t>110.2</t>
   </si>
   <si>
+    <t>Used standard scores to control for age-related improvements</t>
+  </si>
+  <si>
+    <t>Executive loaded working memory and phonological short-term memory</t>
+  </si>
+  <si>
+    <t>d = .65 - .69</t>
+  </si>
+  <si>
+    <t>d = .27 - .97</t>
+  </si>
+  <si>
+    <t>The p-values and effect sizes were only provided for some outcomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se calculó el total de sesiones multiplicando la cantidad de sesiones semanales (4) por la cantidad de semanas (5). Este artículo tiene dos experimentos. This is substudy 1, por lo que se entrarán los datos de ambos experimentos bajo el mismo autor, pero por separado. </t>
+  </si>
+  <si>
+    <t>Los dos estudios de Ecalle et al 2013 no especifican modalidad. Se infiere que fueron grupales, porque menciona que había una asistente presente para atender las dudas que tuvieran los niños. Por otro lado, al igual que en el otro estudio de Ecalle 203, se calculó el total de sesiones multiplicando la cantidad de sesiones semanales por el total de semanas (4x5, respectivamente). This is substudy 2</t>
+  </si>
+  <si>
     <t>Group</t>
   </si>
   <si>
+    <t>Los autores mencionaba que las intervenciones se hicieron diariamente en la escuela y que fueron 8 semanas de intervención</t>
+  </si>
+  <si>
     <t>Messer et al</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Session total, range</t>
+  </si>
+  <si>
+    <t>Percentage of correct responses, range</t>
+  </si>
+  <si>
+    <t>Missing information about instruments and sloppy presentation of results make it hard to determine improvements. Rate of reading (WPM) and spelling show some improvements but hypothesis testing analyses were not performed</t>
+  </si>
+  <si>
+    <t>d = .94</t>
+  </si>
+  <si>
+    <t>Hedges G = .57 - .75</t>
+  </si>
+  <si>
     <t>20 - 30</t>
   </si>
   <si>
@@ -168,12 +382,39 @@
     <t>25 - 30</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>888</t>
+  </si>
+  <si>
+    <t>General comments</t>
+  </si>
+  <si>
     <t>14 - 17</t>
   </si>
   <si>
     <t>3 - 4</t>
   </si>
   <si>
+    <t>n2 = .09 - .15</t>
+  </si>
+  <si>
+    <t>d = 1.5 - 12.1</t>
+  </si>
+  <si>
+    <t>d = .79 - 1.28</t>
+  </si>
+  <si>
+    <t>d = 1.09 - 6.96</t>
+  </si>
+  <si>
+    <t>d = .45 - 1.34</t>
+  </si>
+  <si>
+    <t>d = .40 - .68</t>
+  </si>
+  <si>
     <t>3 - 7</t>
   </si>
   <si>
@@ -204,17 +445,392 @@
     <t>Supervision</t>
   </si>
   <si>
+    <t>Intervention name</t>
+  </si>
+  <si>
+    <t>Instruments to measure cognition</t>
+  </si>
+  <si>
+    <t>Instruments to measure reading skills</t>
+  </si>
+  <si>
+    <t>Random assignment</t>
+  </si>
+  <si>
+    <t>Assessment counterbalancing</t>
+  </si>
+  <si>
+    <t>Variables for group balance</t>
+  </si>
+  <si>
+    <t>Other methodological controls</t>
+  </si>
+  <si>
+    <t>Descriptive statistics provided</t>
+  </si>
+  <si>
+    <t>Mean/Median</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Other descriptive statistics</t>
+  </si>
+  <si>
+    <t>Comments about descriptive statistics</t>
+  </si>
+  <si>
+    <t>Inferential statistics</t>
+  </si>
+  <si>
+    <t>Covariate</t>
+  </si>
+  <si>
+    <t>Effect size provided</t>
+  </si>
+  <si>
+    <t>Mean confidence interval</t>
+  </si>
+  <si>
+    <t>Mean difference confidence interval</t>
+  </si>
+  <si>
+    <t>Other statistical controls</t>
+  </si>
+  <si>
+    <t>Comments inferential statistics</t>
+  </si>
+  <si>
+    <t>Improved cognitive processes</t>
+  </si>
+  <si>
+    <t>Cognitive processes that did not improve</t>
+  </si>
+  <si>
+    <t>Effect size cognition</t>
+  </si>
+  <si>
+    <t>Improved reading skills</t>
+  </si>
+  <si>
+    <t>Reading skills no improvement</t>
+  </si>
+  <si>
+    <t>Effect size reading skills</t>
+  </si>
+  <si>
+    <t>Comments effect on reading skills</t>
+  </si>
+  <si>
+    <t>Comments effect on cognition</t>
+  </si>
+  <si>
     <t>Supervised</t>
   </si>
   <si>
+    <t>Percentage, total</t>
+  </si>
+  <si>
+    <t>Incorporated into the intervention</t>
+  </si>
+  <si>
+    <t>Grapho-syllabic training (GST) and Grapho-phonemic training (GPT)</t>
+  </si>
+  <si>
+    <t>Gates-MacGinitie Reading Test, Words Their Way Elementary Spelling Inventory and Spelling-by-Stage Classroom Organization Chart</t>
+  </si>
+  <si>
+    <t>The effect sizes in this study mean the intervention effect compared to the traditional intervention (group 1) and the regular instruction (group 2), which is interpreted as the speed with which the participant's word frequency reading level improved compared to other the interventions.
+There was other set of analyses but were complicated (for me to interpret) and there was no transparent way to present a summary of the results that would be easily comparable to other studies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 interventions given simultaneously </t>
+  </si>
+  <si>
+    <t>El total de sesiones que ellos reportan (8) no cuadra con la cantidad de sesiones por semana y el total de semanas de intervención (que reportan). No sé si es un error de ellos, pero dice que fueron 8 sesiones en total, de 3 a 4 veces por semanas, por un total de 3 semanas. Participants were native mandarin speakers.</t>
+  </si>
+  <si>
+    <t>Very little control over the number of sessions, frequency, and duration, which were not specified. Not necessarily sessions; more like tutorials/lessons</t>
+  </si>
+  <si>
+    <t>60 lessons were the maximum number of sessions</t>
+  </si>
+  <si>
     <t>Not supervised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPHOT and Omega-Interactive Sentences </t>
+  </si>
+  <si>
+    <t>GraphoGame (Rime-GraphoGame and Rime-Phoneme)</t>
+  </si>
+  <si>
+    <t>PBS KIDS Island</t>
+  </si>
+  <si>
+    <t>GraphoGame and On track ABC</t>
+  </si>
+  <si>
+    <t>Researcher-developed: Computer-based flash-card reading</t>
+  </si>
+  <si>
+    <t>Researcher-developed (no name provided)</t>
+  </si>
+  <si>
+    <t>British Picture Vocabulary Subscale II, BAS II, Test of Word Reading Efficiency, researcher-developed measures</t>
+  </si>
+  <si>
+    <t>researcher-developed measures, Norwegian Vocabulary Test (abbreviated))</t>
+  </si>
+  <si>
+    <t>Flash-card words (researcher-developed measures)</t>
+  </si>
+  <si>
+    <t>Which Picture is the Correct one?, Woodcock Reading Mastery Test-Revised, Wordchains test, Test of Word Reading Efficiency (TOWRE) and a researcher-developed measures (a list of pseudowords).</t>
+  </si>
+  <si>
+    <t>Researcher-developed measures, ODéDys, THaPHo, Peabody Picture Vocabulary Test-Revised</t>
+  </si>
+  <si>
+    <t>ANCOVA, ANOVAs, and Regression</t>
+  </si>
+  <si>
+    <t>Regression analysis</t>
+  </si>
+  <si>
+    <t>Pretest reading skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listening comprehension task, Silent word reading task, aloud word reading and Reading Comprehension. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word recognition, aloud word reading, and Word Spelling. </t>
+  </si>
+  <si>
+    <t>Specific p-value provided</t>
+  </si>
+  <si>
+    <t>phonological skills</t>
+  </si>
+  <si>
+    <t>word reading</t>
+  </si>
+  <si>
+    <t>Phonological skills, word reading</t>
+  </si>
+  <si>
+    <t>Word reading</t>
+  </si>
+  <si>
+    <t>word reading, reading fluency, reading comprehension</t>
+  </si>
+  <si>
+    <t>phonics, phonological skills, vocabulary</t>
+  </si>
+  <si>
+    <t>vocabulary, word reading, spelling, phonological skills</t>
+  </si>
+  <si>
+    <t>Word reading, spelling</t>
+  </si>
+  <si>
+    <t>word reading, Reading comprehension</t>
+  </si>
+  <si>
+    <t>Reading skills (not specified), Spelling</t>
+  </si>
+  <si>
+    <t>Reading comprehension, phonological skills, word reading</t>
+  </si>
+  <si>
+    <t>Word reading, phonological skills</t>
+  </si>
+  <si>
+    <t>Word reading, reading comprehension</t>
+  </si>
+  <si>
+    <t>Reading Fluency</t>
+  </si>
+  <si>
+    <t>Reading comprehension, word recognition</t>
+  </si>
+  <si>
+    <t>reading comprehension, Vocabulary, reading fluency</t>
+  </si>
+  <si>
+    <t>Improved reading skills_coded</t>
+  </si>
+  <si>
+    <t>Reading skills no improvement_coded</t>
+  </si>
+  <si>
+    <t>Blending, Non-word reading</t>
+  </si>
+  <si>
+    <t>Sight-word acquisition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blending CV, Blending VC, Rime articulation and Coda articulation. </t>
+  </si>
+  <si>
+    <t>Word recognition, word reading aloud and word spelling.</t>
+  </si>
+  <si>
+    <t>Word reading aloud</t>
+  </si>
+  <si>
+    <t>Silent word reading, word reading aloud and Reading comprehension</t>
+  </si>
+  <si>
+    <t>Reading and Spelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading comprehension, Passage comprehension, Word decoding, Sight word reading, and Pseudoword reading. </t>
+  </si>
+  <si>
+    <t>Written word recognition, Written word naming, and Phonological awareness</t>
+  </si>
+  <si>
+    <t>Grapho-syllabic training: written word recognition
+Comprehension training: listening comprehension, reading comprehension</t>
+  </si>
+  <si>
+    <t>Rate of reading (WPM), spelling</t>
+  </si>
+  <si>
+    <t>Oral Reading Fluency</t>
+  </si>
+  <si>
+    <t>word identification, reading fluency, listening comprehension (interaction between group and time), reading comprehension (interaction between group and time)</t>
+  </si>
+  <si>
+    <t>High SES: RAN; low SES: letter sound knowledge</t>
+  </si>
+  <si>
+    <t>word reading fluency</t>
+  </si>
+  <si>
+    <t>Lowercase letter knowledge, letter sound awareness, letter sound fluency, letter sequencing, alliterations, phonics, vocabulary, Get ready to Read (instrument)</t>
+  </si>
+  <si>
+    <t>word reading, sentence reading, spelling</t>
+  </si>
+  <si>
+    <t>Phoneme Segmentation Fluency</t>
+  </si>
+  <si>
+    <t>Phoneme segmentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segmenting CV, Segmenting VC, WRAT word reading, Unique words, High N nonwords, Low N nonwords and Letter-sounds. </t>
+  </si>
+  <si>
+    <t>Grapho-syllabic training: listening and reading comprehension
+Comprehension training: word recognition</t>
+  </si>
+  <si>
+    <t>vocabulary, word reading, spelling, phonological awareness, and rhyme awareness</t>
+  </si>
+  <si>
+    <t>Comprehension, Vocabulary, Oral reading rate, reading accuracy</t>
+  </si>
+  <si>
+    <t>Initial Sound Fluency, Letter Naming Fluency, Word Use Fluency), Phoneme Segmentation, Nonsense Word Fluency, and Retell Fluency</t>
+  </si>
+  <si>
+    <t>Phonological awareness, letter name knowledge, reading of words, reading of pseudowords, reading of frequent wods</t>
+  </si>
+  <si>
+    <t>uppercase letter knowledge, uppercase letter naming fluency, lowercase letter naming fluency, rhyming</t>
+  </si>
+  <si>
+    <t>reading fluency, spelling</t>
+  </si>
+  <si>
+    <t>Rapid automatized naming, phonics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phonological skills, phonics, word reading </t>
+  </si>
+  <si>
+    <t>phonics, phonological skills</t>
+  </si>
+  <si>
+    <t>Phonological skills, word reading, phonics</t>
+  </si>
+  <si>
+    <t>reading comprehension, vocabulary, reading fluency</t>
+  </si>
+  <si>
+    <t>The results extracted are only focused on the pre-posttest gains and does not includenot relevant results (other variables).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No inferential statistics wereconducted </t>
+  </si>
+  <si>
+    <t>Pre-test reading skills,age, income, mother's age, mother's education</t>
+  </si>
+  <si>
+    <t>n2 =.33</t>
+  </si>
+  <si>
+    <t>r = Grapho-syllabic training: .80 - .84, Comprehension training: .52 - .88</t>
+  </si>
+  <si>
+    <t>d = Posttest: .22 - 1.01, follow-up: -.30 - 1.01</t>
+  </si>
+  <si>
+    <t>n2 = .06 - .14</t>
+  </si>
+  <si>
+    <t>n2 = High SES: .26, low SES: .21</t>
+  </si>
+  <si>
+    <t>n2 = .064 - .070, d = .35 - .36</t>
+  </si>
+  <si>
+    <t>n2 = .04 - .159</t>
+  </si>
+  <si>
+    <t>Effect size classification</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>medium to large</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comprehension training: .52 - .88</t>
+  </si>
+  <si>
+    <t>Grapho-syllabic training: large, Comprehension training: medium to large</t>
+  </si>
+  <si>
+    <t>small to large</t>
+  </si>
+  <si>
+    <t>small to medium</t>
+  </si>
+  <si>
+    <t>Posttest: small to large, follow-up: small to large</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +843,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -249,19 +872,550 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -435,21 +1589,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:H23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AN23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:AN23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN23">
     <sortCondition ref="A1:A23"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0B078E7E-83E4-453C-8557-B689B2516465}" name="ID" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{3AD873ED-B3D7-417E-A6AB-800F1E5459F4}" name="Author" dataDxfId="6"/>
-    <tableColumn id="23" xr3:uid="{C92854F5-2EF0-4285-B7F6-8C05B4A90195}" name="Session number" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{B30E45D7-CC2B-4FDC-81C4-AB4317E182CE}" name="Session duration" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{19C302C0-56F0-45E0-95EE-BCBDAF18F282}" name="sessions frequency" dataDxfId="3"/>
-    <tableColumn id="26" xr3:uid="{ACEA4A35-6C0A-4701-8F70-24864DBA8770}" name="Modality" dataDxfId="2"/>
-    <tableColumn id="27" xr3:uid="{A06FDE04-A553-4BEF-995A-31322B29A28C}" name="Participants in group modality" dataDxfId="1"/>
-    <tableColumn id="28" xr3:uid="{0FED9BC8-7DB8-4F8E-B677-DADF5940B6CC}" name="Supervision" dataDxfId="0"/>
+  <tableColumns count="40">
+    <tableColumn id="1" xr3:uid="{0B078E7E-83E4-453C-8557-B689B2516465}" name="ID" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{3AD873ED-B3D7-417E-A6AB-800F1E5459F4}" name="Author" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{C92854F5-2EF0-4285-B7F6-8C05B4A90195}" name="Session number" dataDxfId="37"/>
+    <tableColumn id="24" xr3:uid="{B30E45D7-CC2B-4FDC-81C4-AB4317E182CE}" name="Session duration" dataDxfId="36"/>
+    <tableColumn id="25" xr3:uid="{19C302C0-56F0-45E0-95EE-BCBDAF18F282}" name="sessions frequency" dataDxfId="35"/>
+    <tableColumn id="26" xr3:uid="{ACEA4A35-6C0A-4701-8F70-24864DBA8770}" name="Modality" dataDxfId="34"/>
+    <tableColumn id="27" xr3:uid="{A06FDE04-A553-4BEF-995A-31322B29A28C}" name="Participants in group modality" dataDxfId="33"/>
+    <tableColumn id="28" xr3:uid="{0FED9BC8-7DB8-4F8E-B677-DADF5940B6CC}" name="Supervision" dataDxfId="32"/>
+    <tableColumn id="29" xr3:uid="{4D548382-0ABC-4BD6-9A3D-78FCE85DCBC1}" name="Intervention name" dataDxfId="31"/>
+    <tableColumn id="30" xr3:uid="{63FCD5C3-B077-493B-B321-B0604366EB96}" name="Instruments to measure cognition" dataDxfId="30"/>
+    <tableColumn id="31" xr3:uid="{E3A52C0B-9BE7-4A14-93E7-C4247CE91B90}" name="Instruments to measure reading skills" dataDxfId="29"/>
+    <tableColumn id="32" xr3:uid="{0D56973D-C88D-40FE-A90F-B0AFB213AFDF}" name="Random assignment" dataDxfId="28"/>
+    <tableColumn id="33" xr3:uid="{ECFDDC08-D3B7-4CF9-AF2D-BA1AAE9641F6}" name="Assessment counterbalancing" dataDxfId="27"/>
+    <tableColumn id="34" xr3:uid="{EE5CE2B4-6D44-44A0-BC90-566EB9520766}" name="Variables for group balance" dataDxfId="26"/>
+    <tableColumn id="37" xr3:uid="{C28C160E-D7AE-41F1-9FB7-C3E66D709720}" name="Other methodological controls" dataDxfId="25"/>
+    <tableColumn id="38" xr3:uid="{2EA382FB-29FE-4AAB-A2D4-55C13414BFF5}" name="Descriptive statistics provided" dataDxfId="24"/>
+    <tableColumn id="39" xr3:uid="{09505FCD-0E9E-4883-A35E-0564AA34BA56}" name="Mean/Median" dataDxfId="23"/>
+    <tableColumn id="40" xr3:uid="{484DDF92-F6A0-4359-8958-DC5B1C8A3B0C}" name="Standard deviation" dataDxfId="22"/>
+    <tableColumn id="41" xr3:uid="{55D2984D-1B81-4C5D-887F-785B42549436}" name="Mean confidence interval" dataDxfId="21"/>
+    <tableColumn id="42" xr3:uid="{1C5ABDAC-5E8F-4586-AF3F-5CE38E434290}" name="Other descriptive statistics" dataDxfId="20"/>
+    <tableColumn id="57" xr3:uid="{C48DCD7B-4527-4E53-A3F7-E60E0ECEF558}" name="Comments about descriptive statistics" dataDxfId="19"/>
+    <tableColumn id="44" xr3:uid="{7A4931EC-DAB2-43FD-9563-B41C63AF994C}" name="Inferential statistics" dataDxfId="18"/>
+    <tableColumn id="45" xr3:uid="{04FD368E-6727-4A16-B432-6055946ADB4E}" name="Covariate" dataDxfId="17"/>
+    <tableColumn id="46" xr3:uid="{002B09FC-42A5-4B9E-B00B-4247469ED640}" name="Specific p-value provided" dataDxfId="16"/>
+    <tableColumn id="47" xr3:uid="{2491D4F3-A98E-4ED6-9CC0-5BEBA0AED5A2}" name="Effect size provided" dataDxfId="15"/>
+    <tableColumn id="48" xr3:uid="{ED100DE6-09FF-4604-99D6-73681EB7237F}" name="Mean difference confidence interval" dataDxfId="14"/>
+    <tableColumn id="49" xr3:uid="{51DB6773-4D14-4AE1-9DA6-3C452E8BD712}" name="Other statistical controls" dataDxfId="13"/>
+    <tableColumn id="58" xr3:uid="{5B74B444-7863-49DC-BECA-49FEE05F9984}" name="Comments inferential statistics" dataDxfId="12"/>
+    <tableColumn id="50" xr3:uid="{E36D3572-9344-404D-AEED-4C18E7A993EF}" name="Improved cognitive processes" dataDxfId="11"/>
+    <tableColumn id="51" xr3:uid="{2B520559-FCB3-4512-B091-68EA56AAEE21}" name="Cognitive processes that did not improve" dataDxfId="10"/>
+    <tableColumn id="52" xr3:uid="{1EA75320-37D8-4F15-940E-B6A10594C3A3}" name="Effect size cognition" dataDxfId="9"/>
+    <tableColumn id="59" xr3:uid="{D5BEAA29-1A8C-40F5-9AC8-5637860CE237}" name="Comments effect on cognition" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{05BA5D65-9865-E24C-8C24-D3F101DAAF39}" name="Improved reading skills" dataDxfId="7"/>
+    <tableColumn id="53" xr3:uid="{C933BD5B-B918-4F2D-B8F7-CD8E7A132A17}" name="Improved reading skills_coded" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{7FF23964-25F2-9E4E-A060-98AF4F47BE84}" name="Reading skills no improvement" dataDxfId="5"/>
+    <tableColumn id="54" xr3:uid="{F39DD7A1-CBC3-4AF0-B362-68FFD32F347B}" name="Reading skills no improvement_coded" dataDxfId="4"/>
+    <tableColumn id="55" xr3:uid="{A6F391AD-5850-47C2-9D08-4CFA06D01676}" name="Effect size reading skills" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{8C25F0B5-667D-0C43-963E-42642928D327}" name="Effect size classification" dataDxfId="2"/>
+    <tableColumn id="60" xr3:uid="{6050F297-C3B7-4DDE-A740-5139D8EAF8F5}" name="Comments effect on reading skills" dataDxfId="1"/>
+    <tableColumn id="61" xr3:uid="{C3B05082-6C97-4BD7-B093-5FB9EEC21E36}" name="General comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -741,6 +1931,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC0D8D7-AF76-455B-A1D5-F5733B28A0CC}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -768,205 +1970,763 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:AR23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="6"/>
-    <col min="10" max="10" width="68.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="28.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="6"/>
-    <col min="14" max="14" width="9" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="6"/>
+    <col min="9" max="9" width="90.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="192.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="56.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="61.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="33.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="57.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="51.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="118.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="61" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="52.33203125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="47.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="28.5" style="2" customWidth="1"/>
+    <col min="36" max="36" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="39" style="8" customWidth="1"/>
+    <col min="38" max="38" width="15.5" style="2" customWidth="1"/>
+    <col min="39" max="39" width="25.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="255.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.83203125" style="7"/>
+    <col min="42" max="42" width="68.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="28.5" style="2" customWidth="1"/>
+    <col min="45" max="45" width="8.83203125" style="7"/>
+    <col min="46" max="46" width="9" style="7" customWidth="1"/>
+    <col min="47" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+        <v>134</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2">
         <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2">
         <v>888</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+        <v>172</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2">
+        <v>888</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="2">
+        <v>888</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="3"/>
+      <c r="V2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2">
         <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2">
+        <v>888</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" s="2">
+        <v>888</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="3"/>
+      <c r="V3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AK3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G4" s="2">
         <v>888</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="2">
+        <v>888</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="2">
+        <v>888</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>888</v>
+      </c>
+      <c r="R4" s="2">
+        <v>888</v>
+      </c>
+      <c r="S4" s="2">
+        <v>888</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="3"/>
+      <c r="V4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK4" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="7"/>
+      <c r="AR4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E5" s="3">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G5" s="2">
         <v>888</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="2">
+        <v>888</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="2">
+        <v>888</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="3"/>
+      <c r="V5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG5" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AK5" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AP5" s="7"/>
+      <c r="AQ5" s="7"/>
+      <c r="AR5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="2">
+        <v>888</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" s="2">
+        <v>888</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" s="3"/>
+      <c r="V6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK6" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="AL6" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="AM6" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="AN6" s="3"/>
+      <c r="AP6" s="7"/>
+      <c r="AQ6" s="7"/>
+      <c r="AR6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -974,464 +2734,1862 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="E7" s="3">
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G7" s="2">
         <v>888</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="2">
+        <v>888</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="2">
+        <v>888</v>
+      </c>
+      <c r="O7" s="2">
+        <v>888</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="3"/>
+      <c r="V7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI7" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="AL7" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E8" s="3">
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G8" s="2">
         <v>888</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J8" s="2">
+        <v>888</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L8" s="2">
+        <v>888</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N8" s="2">
+        <v>888</v>
+      </c>
+      <c r="O8" s="2">
+        <v>888</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="2">
+        <v>888</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" s="2">
+        <v>888</v>
+      </c>
+      <c r="W8" s="2">
+        <v>888</v>
+      </c>
+      <c r="X8" s="2">
+        <v>888</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>888</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK8" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL8" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN8" s="3"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2">
+        <v>888</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="2">
+        <v>888</v>
+      </c>
+      <c r="N9" s="2">
+        <v>888</v>
+      </c>
+      <c r="O9" s="2">
+        <v>888</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S9" s="2">
+        <v>888</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="V9" s="2">
+        <v>888</v>
+      </c>
+      <c r="W9" s="2">
+        <v>888</v>
+      </c>
+      <c r="X9" s="2">
+        <v>888</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>888</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL9" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G10" s="2">
         <v>888</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+        <v>172</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="2">
+        <v>888</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="2">
+        <v>888</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T10" s="2">
+        <v>888</v>
+      </c>
+      <c r="U10" s="3"/>
+      <c r="V10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AI10" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK10" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="7"/>
+      <c r="AR10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="2">
+        <v>888</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N11" s="2">
+        <v>888</v>
+      </c>
+      <c r="O11" s="2">
+        <v>888</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="3"/>
+      <c r="V11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG11" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI11" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AK11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL11" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="7"/>
+      <c r="AR11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="C12" s="3">
         <v>93.4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J12" s="2">
+        <v>888</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="2">
+        <v>888</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="3"/>
+      <c r="V12" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="W12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="X12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG12" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK12" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AL12" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AM12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="7"/>
+      <c r="AR12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E13" s="3">
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G13" s="2">
         <v>888</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="J13" s="2">
+        <v>888</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13" s="2">
+        <v>888</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U13" s="3"/>
+      <c r="V13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK13" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL13" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AP13" s="7"/>
+      <c r="AQ13" s="7"/>
+      <c r="AR13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C14" s="3">
         <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="J14" s="2">
+        <v>888</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="2">
+        <v>888</v>
+      </c>
+      <c r="M14" s="2">
+        <v>888</v>
+      </c>
+      <c r="N14" s="2">
+        <v>888</v>
+      </c>
+      <c r="O14" s="2">
+        <v>888</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S14" s="2">
+        <v>888</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U14" s="3"/>
+      <c r="V14" s="2">
+        <v>888</v>
+      </c>
+      <c r="W14" s="2">
+        <v>888</v>
+      </c>
+      <c r="X14" s="2">
+        <v>888</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>888</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG14" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK14" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL14" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7"/>
+      <c r="AR14" s="7"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C15" s="3">
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J15" s="2">
+        <v>888</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" s="2">
+        <v>888</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U15" s="3"/>
+      <c r="V15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK15" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="AL15" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP15" s="7"/>
+      <c r="AQ15" s="7"/>
+      <c r="AR15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J16" s="2">
+        <v>888</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O16" s="2">
+        <v>888</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U16" s="3"/>
+      <c r="V16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH16" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK16" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL16" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP16" s="7"/>
+      <c r="AQ16" s="7"/>
+      <c r="AR16" s="7"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C17" s="3">
         <v>60</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="E17" s="3">
         <v>5</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J17" s="2">
+        <v>888</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U17" s="3"/>
+      <c r="V17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD17" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK17" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN17" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP17" s="7"/>
+      <c r="AQ17" s="7"/>
+      <c r="AR17" s="7"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G18" s="2">
         <v>888</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="2">
+        <v>888</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="2">
+        <v>888</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" s="2">
+        <v>888</v>
+      </c>
+      <c r="O18" s="2">
+        <v>888</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK18" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL18" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="AP18" s="7"/>
+      <c r="AQ18" s="7"/>
+      <c r="AR18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J19" s="2">
+        <v>888</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="2">
+        <v>888</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" s="2">
+        <v>888</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG19" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI19" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK19" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL19" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AM19" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AN19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP19" s="7"/>
+      <c r="AQ19" s="7"/>
+      <c r="AR19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3">
         <v>25</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G20" s="2">
         <v>888</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J20" s="2">
+        <v>888</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O20" s="2">
+        <v>888</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="3"/>
+      <c r="V20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE20" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK20" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL20" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="3"/>
+      <c r="AP20" s="7"/>
+      <c r="AQ20" s="7"/>
+      <c r="AR20" s="7"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E21" s="3">
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G21" s="2">
         <v>888</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J21" s="2">
+        <v>888</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" s="2">
+        <v>888</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U21" s="3"/>
+      <c r="V21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE21" s="2">
+        <v>888</v>
+      </c>
+      <c r="AF21" s="3"/>
+      <c r="AG21" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AH21" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AI21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK21" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL21" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AM21" s="3"/>
+      <c r="AN21" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="AP21" s="7"/>
+      <c r="AQ21" s="7"/>
+      <c r="AR21" s="7"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" s="2">
+        <v>888</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>888</v>
+      </c>
+      <c r="AE22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG22" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AI22" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="AK22" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL22" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AQ22" s="7"/>
+      <c r="AR22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1442,12 +4600,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1597,15 +4752,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1630,17 +4796,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>